<commit_message>
added log for cpu_windows
</commit_message>
<xml_diff>
--- a/emagevision/cpu_each_user_emagevision.xlsx
+++ b/emagevision/cpu_each_user_emagevision.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>date_cpu</t>
   </si>
@@ -218,6 +218,168 @@
   </si>
   <si>
     <t>Sep_6_12</t>
+  </si>
+  <si>
+    <t>Sep_6_18</t>
+  </si>
+  <si>
+    <t>Sep_7_0</t>
+  </si>
+  <si>
+    <t>Sep_7_6</t>
+  </si>
+  <si>
+    <t>Sep_7_12</t>
+  </si>
+  <si>
+    <t>Sep_7_18</t>
+  </si>
+  <si>
+    <t>Sep_8_0</t>
+  </si>
+  <si>
+    <t>Sep_8_6</t>
+  </si>
+  <si>
+    <t>Sep_8_12</t>
+  </si>
+  <si>
+    <t>Sep_8_18</t>
+  </si>
+  <si>
+    <t>Sep_9_0</t>
+  </si>
+  <si>
+    <t>Sep_9_6</t>
+  </si>
+  <si>
+    <t>Sep_9_12</t>
+  </si>
+  <si>
+    <t>Sep_9_18</t>
+  </si>
+  <si>
+    <t>Sep_10_0</t>
+  </si>
+  <si>
+    <t>Sep_10_6</t>
+  </si>
+  <si>
+    <t>Sep_10_12</t>
+  </si>
+  <si>
+    <t>Sep_10_18</t>
+  </si>
+  <si>
+    <t>Sep_11_0</t>
+  </si>
+  <si>
+    <t>Sep_11_6</t>
+  </si>
+  <si>
+    <t>Sep_11_12</t>
+  </si>
+  <si>
+    <t>Sep_11_18</t>
+  </si>
+  <si>
+    <t>Sep_12_0</t>
+  </si>
+  <si>
+    <t>Sep_12_6</t>
+  </si>
+  <si>
+    <t>Sep_12_12</t>
+  </si>
+  <si>
+    <t>Sep_12_18</t>
+  </si>
+  <si>
+    <t>Sep_13_0</t>
+  </si>
+  <si>
+    <t>Sep_13_6</t>
+  </si>
+  <si>
+    <t>Sep_13_12</t>
+  </si>
+  <si>
+    <t>Sep_13_18</t>
+  </si>
+  <si>
+    <t>Sep_14_0</t>
+  </si>
+  <si>
+    <t>Sep_14_12</t>
+  </si>
+  <si>
+    <t>Sep_14_18</t>
+  </si>
+  <si>
+    <t>Sep_15_0</t>
+  </si>
+  <si>
+    <t>Sep_15_6</t>
+  </si>
+  <si>
+    <t>Sep_15_12</t>
+  </si>
+  <si>
+    <t>Sep_15_18</t>
+  </si>
+  <si>
+    <t>Sep_16_0</t>
+  </si>
+  <si>
+    <t>Sep_16_6</t>
+  </si>
+  <si>
+    <t>Sep_16_12</t>
+  </si>
+  <si>
+    <t>Sep_16_18</t>
+  </si>
+  <si>
+    <t>Sep_17_0</t>
+  </si>
+  <si>
+    <t>Sep_17_6</t>
+  </si>
+  <si>
+    <t>Sep_17_12</t>
+  </si>
+  <si>
+    <t>Sep_17_18</t>
+  </si>
+  <si>
+    <t>Sep_18_0</t>
+  </si>
+  <si>
+    <t>Sep_18_6</t>
+  </si>
+  <si>
+    <t>Sep_18_12</t>
+  </si>
+  <si>
+    <t>Sep_18_18</t>
+  </si>
+  <si>
+    <t>Sep_19_0</t>
+  </si>
+  <si>
+    <t>Sep_19_6</t>
+  </si>
+  <si>
+    <t>Sep_19_12</t>
+  </si>
+  <si>
+    <t>Sep_19_18</t>
+  </si>
+  <si>
+    <t>Sep_20_0</t>
+  </si>
+  <si>
+    <t>Sep_20_6</t>
   </si>
 </sst>
 </file>
@@ -549,7 +711,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3093,6 +3255,2544 @@
         <v>0</v>
       </c>
     </row>
+    <row r="55" spans="1:15">
+      <c r="A55" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>3.3</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>3.3</v>
+      </c>
+      <c r="H56">
+        <v>0.1</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>3.3</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
+      <c r="A58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>3.3</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>3.3</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
+      <c r="A60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>3.3</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
+      <c r="A61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>3.3</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
+      <c r="A62" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>3.3</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
+      <c r="A63" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>3.3</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>3.2</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
+      <c r="A65" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>3.2</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
+      <c r="A66" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>3.2</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15">
+      <c r="A67" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>3.1</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
+      <c r="A68" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <v>0</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
+      <c r="A69" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>3</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69">
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+      <c r="O69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
+      <c r="A70" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+      <c r="N70">
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="A71" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>3</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
+      <c r="A72" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>3</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
+      <c r="A73" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
+      <c r="A74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>2.8</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
+      <c r="A75" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>3.1</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+      <c r="O75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
+      <c r="A76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0.1</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>3.1</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
+      </c>
+      <c r="O76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="A77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>3.1</v>
+      </c>
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77">
+        <v>10.1</v>
+      </c>
+      <c r="O77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>3.1</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>9.9</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
+      <c r="A79" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>3.1</v>
+      </c>
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="O79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
+      <c r="A80" t="s">
+        <v>93</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0.1</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>3.1</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
+      <c r="A81" t="s">
+        <v>94</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>3.1</v>
+      </c>
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+      <c r="N81">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
+      <c r="A82" t="s">
+        <v>95</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>3.1</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <v>9.9</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
+      <c r="A83" t="s">
+        <v>96</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>3.1</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
+      <c r="A84" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0.1</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>3.1</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="N84">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
+      <c r="A85" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
+      <c r="A86" t="s">
+        <v>99</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <v>0</v>
+      </c>
+      <c r="N86">
+        <v>0</v>
+      </c>
+      <c r="O86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
+      <c r="A87" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+      <c r="N87">
+        <v>0</v>
+      </c>
+      <c r="O87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
+      <c r="A88" t="s">
+        <v>101</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+      <c r="N88">
+        <v>0</v>
+      </c>
+      <c r="O88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
+      <c r="A89" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>2.8</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+      <c r="N89">
+        <v>0</v>
+      </c>
+      <c r="O89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
+      <c r="A90" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>1.6</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+      <c r="N90">
+        <v>0</v>
+      </c>
+      <c r="O90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
+      <c r="A91" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>1.6</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <v>0</v>
+      </c>
+      <c r="N91">
+        <v>0</v>
+      </c>
+      <c r="O91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
+      <c r="A92" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>7.3</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>1.6</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <v>0</v>
+      </c>
+      <c r="N92">
+        <v>0</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15">
+      <c r="A93" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>9.1</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>1.6</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>0</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+      <c r="N93">
+        <v>0</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15">
+      <c r="A94" t="s">
+        <v>107</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>1.7</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94">
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+      <c r="N94">
+        <v>0</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
+      <c r="A95" t="s">
+        <v>108</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>1.7</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95">
+        <v>0</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="N95">
+        <v>0</v>
+      </c>
+      <c r="O95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
+      <c r="A96" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>1.7</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+      <c r="O96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
+      <c r="A97" t="s">
+        <v>110</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>1.7</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
+      <c r="A98" t="s">
+        <v>111</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>1.7</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98">
+        <v>0</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
+      <c r="A99" t="s">
+        <v>112</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>1.7</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
+      <c r="A100" t="s">
+        <v>113</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>1.8</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+      <c r="N100">
+        <v>0</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
+      <c r="A101" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>1.7</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101">
+        <v>0</v>
+      </c>
+      <c r="N101">
+        <v>0</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
+      <c r="A102" t="s">
+        <v>115</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>1.8</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
+        <v>0</v>
+      </c>
+      <c r="N102">
+        <v>0</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
+      <c r="A103" t="s">
+        <v>116</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>1.8</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <v>0</v>
+      </c>
+      <c r="N103">
+        <v>0</v>
+      </c>
+      <c r="O103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
+      <c r="A104" t="s">
+        <v>117</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>1.8</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
+        <v>0</v>
+      </c>
+      <c r="N104">
+        <v>0</v>
+      </c>
+      <c r="O104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15">
+      <c r="A105" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>1.8</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <v>0</v>
+      </c>
+      <c r="N105">
+        <v>0</v>
+      </c>
+      <c r="O105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15">
+      <c r="A106" t="s">
+        <v>119</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>1.8</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106">
+        <v>0</v>
+      </c>
+      <c r="O106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15">
+      <c r="A107" t="s">
+        <v>120</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>1.8</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107">
+        <v>0</v>
+      </c>
+      <c r="N107">
+        <v>0</v>
+      </c>
+      <c r="O107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15">
+      <c r="A108" t="s">
+        <v>121</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>1.8</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108">
+        <v>0</v>
+      </c>
+      <c r="N108">
+        <v>0</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>